<commit_message>
storing title data in db
</commit_message>
<xml_diff>
--- a/test_tituly.xlsx
+++ b/test_tituly.xlsx
@@ -9,24 +9,34 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="8708"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="7852"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>ADM_REC</t>
   </si>
   <si>
+    <t>CALLNO</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
     <t>ISBN</t>
   </si>
   <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
     <t>000000002</t>
   </si>
   <si>
@@ -78,13 +88,22 @@
     <t>Abecední seznam obcí a jejich částí s příslušnými dodávacími poštami v ČSSR - 1964.1. p</t>
   </si>
   <si>
-    <t>CALLNO</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Author</t>
+    <t>000000008</t>
+  </si>
+  <si>
+    <t>Abecední věcný rejstřík k desetinnému třídění používanému v Ekonomicko-matematických a</t>
+  </si>
+  <si>
+    <t>000000009</t>
+  </si>
+  <si>
+    <t>Kalkulationsunterlagen f.d. Leistung beim Rücken mit Forsttraktoren und beim Reisten auf kurze Dist</t>
+  </si>
+  <si>
+    <t>Abegg, Bruno</t>
+  </si>
+  <si>
+    <t>YYY</t>
   </si>
 </sst>
 </file>
@@ -402,107 +421,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="105.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>